<commit_message>
Implementação bd e iniciando TKinter
</commit_message>
<xml_diff>
--- a/tabelaExcel.xlsx
+++ b/tabelaExcel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,55 +458,55 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>varistor</t>
+          <t>tv</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>componente eletrônico</t>
+          <t>eletrônico</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.35</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>lapis</t>
+          <t>carregador</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>item de escola</t>
+          <t>eletrônico</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>cola</t>
+          <t>varistor</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>item de escola</t>
+          <t>componente eletrônico</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="5">
@@ -524,7 +524,151 @@
         </is>
       </c>
       <c r="D5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>cola</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>50</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>item de escola</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>lapis</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>10</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>item de escola</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>caneta</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>80</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>item de escola</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>varistor</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>componente eletrônico</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>lapis</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>item de escola</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>cola</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>50</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>item de escola</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>lapis</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>item de escola</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>caneta</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>80</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>item de escola</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>3.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criação da navegação entre janelas
</commit_message>
<xml_diff>
--- a/tabelaExcel.xlsx
+++ b/tabelaExcel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,29 +512,29 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>lapis</t>
+          <t>varistor</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>item de escola</t>
+          <t>componente eletrônico</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>cola</t>
+          <t>lapis</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -548,11 +548,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>lapis</t>
+          <t>cola</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -560,17 +560,17 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>caneta</t>
+          <t>lapis</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -578,53 +578,53 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3.9</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>varistor</t>
+          <t>caneta</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>componente eletrônico</t>
+          <t>item de escola</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.35</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>lapis</t>
+          <t>varistor</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>item de escola</t>
+          <t>componente eletrônico</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>cola</t>
+          <t>lapis</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -638,11 +638,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>lapis</t>
+          <t>cola</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -650,17 +650,17 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>caneta</t>
+          <t>lapis</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -668,53 +668,53 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3.9</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>varistor</t>
+          <t>caneta</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>componente eletrônico</t>
+          <t>item de escola</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.35</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>lapis</t>
+          <t>varistor</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>item de escola</t>
+          <t>componente eletrônico</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>cola</t>
+          <t>lapis</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -728,11 +728,11 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>lapis</t>
+          <t>cola</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -740,24 +740,42 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>lapis</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>10</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>item de escola</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>caneta</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="B19" t="n">
         <v>80</v>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>item de escola</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>item de escola</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
         <v>3.9</v>
       </c>
     </row>

</xml_diff>